<commit_message>
Fri Jan 19 16:31:22 CST 2024
</commit_message>
<xml_diff>
--- a/计划/2024学习计划.xlsx
+++ b/计划/2024学习计划.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="28">
   <si>
     <t>早餐</t>
   </si>
@@ -105,44 +105,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>1音视频/10技术书/复习1/1习题</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1音频/1视频/10技术书/1习题</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/1视频/10技术书/1习题</t>
     </r>
   </si>
   <si>
@@ -917,7 +879,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -955,9 +917,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1393,8 +1352,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -1901,8 +1860,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -2409,8 +2368,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -2917,8 +2876,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -3319,8 +3278,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3412,8 +3371,8 @@
       <c r="G5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>8</v>
+      <c r="H5" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -3425,8 +3384,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -3439,7 +3398,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3471,17 +3430,17 @@
         <v>0</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="14" t="s">
         <v>11</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="15" t="s">
-        <v>12</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -3491,23 +3450,23 @@
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>15</v>
-      </c>
       <c r="E11" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="14" t="s">
         <v>16</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3518,8 +3477,8 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="15" t="s">
-        <v>18</v>
+      <c r="F12" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -3529,7 +3488,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>4</v>
@@ -3555,25 +3514,25 @@
         <v>6</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="G14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3605,10 +3564,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -3621,7 +3580,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -3675,22 +3634,22 @@
         <v>6</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -3991,8 +3950,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -4499,8 +4458,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -5007,8 +4966,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -5515,8 +5474,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -6024,8 +5983,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -6532,8 +6491,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -7040,8 +6999,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -7548,8 +7507,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">

</xml_diff>

<commit_message>
Fri  7 Mar 2025 10:58:33 CST
</commit_message>
<xml_diff>
--- a/计划/2024学习计划.xlsx
+++ b/计划/2024学习计划.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="45">
   <si>
     <t>早餐</t>
   </si>
@@ -193,6 +193,52 @@
   </si>
   <si>
     <t>切片面包</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/1视频/10技术书/1习题</t>
+    </r>
   </si>
   <si>
     <r>
@@ -2394,25 +2440,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -2504,25 +2550,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2602,25 +2648,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2700,25 +2746,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2774,13 +2820,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -3410,25 +3456,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -3520,25 +3566,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3618,25 +3664,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3716,25 +3762,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3790,13 +3836,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4966,8 +5012,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5151,8 +5197,8 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>35</v>
+      <c r="B13" s="15" t="s">
+        <v>7</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>35</v>
@@ -5250,25 +5296,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5348,25 +5394,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5422,13 +5468,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -5550,25 +5596,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5660,25 +5706,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5758,25 +5804,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5856,25 +5902,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5930,13 +5976,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -6061,25 +6107,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -6136,7 +6182,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>11</v>
@@ -6151,7 +6197,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="11" t="s">
@@ -6181,25 +6227,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6210,7 +6256,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>23</v>
@@ -6285,25 +6331,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6383,7 +6429,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>4</v>
@@ -6554,7 +6600,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -6587,25 +6633,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -6697,25 +6743,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6761,10 +6807,10 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -6778,13 +6824,13 @@
         <v>31</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -6795,16 +6841,16 @@
         <v>2</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -6815,25 +6861,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6843,7 +6889,7 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -6915,25 +6961,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6989,13 +7035,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -7625,25 +7671,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -7735,25 +7781,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7833,25 +7879,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7931,25 +7977,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8005,13 +8051,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">

</xml_diff>